<commit_message>
update subject creation: - adds inline-create to streamline process of adding a data subject to a new form; - updates instructions to user around data subjects; - slight modifications to ODK example forms.
</commit_message>
<xml_diff>
--- a/tests/Files/ExampleOdk.xlsx
+++ b/tests/Files/ExampleOdk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Projects/Packages/laravel-odk-link/tests/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57779A6-DBA7-AC43-91F1-A6695D2B49CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0494D05-357D-D44A-B72A-369D64D95591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8500" yWindow="-25280" windowWidth="32600" windowHeight="17560" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24240" yWindow="-28300" windowWidth="51200" windowHeight="28300" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
   <si>
     <t>type</t>
   </si>
@@ -147,27 +147,15 @@
     <t>What is your name?</t>
   </si>
   <si>
-    <t>select_one faculty</t>
-  </si>
-  <si>
     <t>faculty</t>
   </si>
   <si>
-    <t>Which faculty are you a part of?</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
-    <t>select_one status</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>Are you a student, or member of staff?</t>
-  </si>
-  <si>
     <t>Faculty of Business, Law and Art</t>
   </si>
   <si>
@@ -237,12 +225,6 @@
     <t>select_one yn</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
     <t>coffee</t>
   </si>
   <si>
@@ -361,9 +343,6 @@
   </si>
   <si>
     <t>${photo_yn}="1"</t>
-  </si>
-  <si>
-    <t>When did you start in your current role at the University?</t>
   </si>
   <si>
     <t>age</t>
@@ -687,24 +666,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -732,7 +711,6 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1283,11 +1261,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1427,232 +1405,174 @@
         <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>118</v>
+      <c r="I9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="31" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="31" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>78</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="A13:D13">
+  <conditionalFormatting sqref="A10:D10">
     <cfRule type="expression" dxfId="8" priority="1">
-      <formula>NOT(ISERROR(SEARCH("Begin Repeat",A13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Begin Repeat",A10)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="7" priority="2">
-      <formula>NOT(ISERROR(SEARCH("Begin Group",A13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Begin Group",A10)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="6" priority="3">
-      <formula>$A13 = "calculate"</formula>
+      <formula>$A10 = "calculate"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$A13 = "begin group"</formula>
+      <formula>$A10 = "begin group"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>$A13 = "end group"</formula>
+      <formula>$A10 = "end group"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="3" priority="6">
-      <formula>$A13 = "begin repeat"</formula>
+      <formula>$A10 = "begin repeat"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="2" priority="7">
-      <formula>$A13 = "end repeat"</formula>
+      <formula>$A10 = "end repeat"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="1" priority="8">
-      <formula>$A13 = "note"</formula>
+      <formula>$A10 = "note"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13:D13">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>$A13 = "begin repeat"</formula>
+      <formula>$A10 = "begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1690,248 +1610,248 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B15" s="14">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
       </c>
       <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="C19" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="C21" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C25" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="25"/>
+      <c r="A27" s="24"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C10:C18">
@@ -1977,10 +1897,10 @@
     </row>
     <row r="2" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D2">
         <v>20171113</v>

</xml_diff>